<commit_message>
beta 1.3 add scale
</commit_message>
<xml_diff>
--- a/交付表格.xlsx
+++ b/交付表格.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="321">
   <si>
     <t>检查类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1201,6 +1201,27 @@
   </si>
   <si>
     <t>两侧胸廓对称无畸形两侧肺野透亮度正常未见异常密度影。两肺纹理清晰无增深、变形。两肺门无增大、增浓边缘清晰。双横膈面光整，两侧肋膈角清晰锐利。心影大小形态未见异常。纵隔居中无增宽。</t>
+  </si>
+  <si>
+    <t>脾脏肋下未角虫及</t>
+  </si>
+  <si>
+    <t>肺活埕小于2600肺活适减低秒用力吐气量小于2200秒用力吐气童减低</t>
+  </si>
+  <si>
+    <t>双侧乳腺组织厚度正常内部回声欠均匀局部导菅轻度增宽右侧乳腺内上象限可见边界清晰的低回声结节大小约5X3刑n。CD血流未见明显异常</t>
+  </si>
+  <si>
+    <t>子宫形态大小正常肌层回声均匀内膜线显示清晰厚度正常范围，宫颈长度正常</t>
+  </si>
+  <si>
+    <t>双侧卵巢显示清晰形态大小正常CD门血流显示正常</t>
+  </si>
+  <si>
+    <t>颈椎生理曲度正常椎体骨质、椎间隙及附件骨结构正常声</t>
+  </si>
+  <si>
+    <t>两侧胸廓对称无畸形两侧肺野透亮度正常末见异常密度影。两肺纹理清晰无增深、变形l两肺门无增大无增浓鹫边缘清晰。双横膈面光整两侧肋膈角清晰锐利。心影大小形态未见异常。纵隔居中无增宽。</t>
   </si>
 </sst>
 </file>

</xml_diff>